<commit_message>
made some revision for generator, added auto LC of the property name, and added new deployment scripts.
</commit_message>
<xml_diff>
--- a/form_templates.xlsx
+++ b/form_templates.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>FriendlyName</t>
   </si>
@@ -120,13 +120,19 @@
   </si>
   <si>
     <t>eatFish</t>
+  </si>
+  <si>
+    <t>Included column in table view</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +144,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -187,14 +201,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -203,8 +215,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -483,157 +500,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27:F28"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" style="6" customWidth="1"/>
     <col min="3" max="3" width="47.28515625" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-    <col min="8" max="8" width="42.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" customWidth="1"/>
+    <col min="9" max="9" width="42.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="b">
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>5</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>25</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>4</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>29</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>6</v>
       </c>
     </row>

</xml_diff>